<commit_message>
Archivos de input para switch
</commit_message>
<xml_diff>
--- a/Costos/Resultados LCOE asociados a Geotérmica Flash - Municipio de VILLAMARIA - 1_7_2020.xlsx
+++ b/Costos/Resultados LCOE asociados a Geotérmica Flash - Municipio de VILLAMARIA - 1_7_2020.xlsx
@@ -1,10 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicoquintero/Documents/Investigacion andes-EDF/Switch/Sin título/Costos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA387A0-23F9-9C4A-8A47-B838DDE3BD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Página 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -113,11 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,13 +155,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -478,23 +494,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Página 1"/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
-    <col min="4" max="4" width="50.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.83203125" customWidth="1"/>
-    <col min="6" max="6" width="50.83203125" customWidth="1"/>
-    <col min="7" max="7" width="50.83203125" customWidth="1"/>
+    <col min="1" max="7" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -516,7 +529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -527,18 +540,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>8.077325998188481</v>
+        <v>8.0773259981884813</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -549,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -560,18 +573,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>340.4554868</v>
+        <v>340.45548680000002</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -582,18 +595,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9">
-        <v>357.1259788337721</v>
+        <v>357.12597883377208</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -604,29 +617,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>1621.608773741756</v>
+        <v>1621.6087737417561</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12">
-        <v>7207698.299707128</v>
+        <v>7207698.2997071277</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -637,18 +650,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14">
-        <v>5.13852</v>
+        <v>5.1385199999999998</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -659,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -670,7 +683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -681,7 +694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -692,7 +705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -703,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -714,22 +727,38 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21">
-        <v>99.75383516413753</v>
+        <v>99.753835164137527</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A4C92F77D51DB34BB66DB547BA261888" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="036d0ed6745d5cb6fc93e88a90c24f29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3901be2b-e0aa-425f-8ecd-05b022f3c304" xmlns:ns3="1d72c402-e5ab-4c37-8652-a8939ba1b122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8e2230f21ddac050465166b7244a911" ns2:_="" ns3:_="">
     <xsd:import namespace="3901be2b-e0aa-425f-8ecd-05b022f3c304"/>
@@ -894,29 +923,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7184C3A0-3566-4684-8AD3-46F65BCF8EF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A84BB6D6-C314-4199-9162-6535B58A2E67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DF8926-764B-4C14-A0B5-D396CB4867E9}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A84BB6D6-C314-4199-9162-6535B58A2E67}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7184C3A0-3566-4684-8AD3-46F65BCF8EF0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65DF8926-764B-4C14-A0B5-D396CB4867E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3901be2b-e0aa-425f-8ecd-05b022f3c304"/>
+    <ds:schemaRef ds:uri="1d72c402-e5ab-4c37-8652-a8939ba1b122"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>